<commit_message>
now it can use
</commit_message>
<xml_diff>
--- a/plot/plotConfig.xlsx
+++ b/plot/plotConfig.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6148" yWindow="0" windowWidth="14317" windowHeight="6729"/>
+    <workbookView xWindow="7172" yWindow="0" windowWidth="14317" windowHeight="6729"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>act_weight</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -157,10 +157,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>规格</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>plot_dist_absolute</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -206,6 +202,18 @@
   </si>
   <si>
     <t>宽度相对量分布</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吨位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百分比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>规格分布</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -617,7 +625,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
@@ -677,10 +685,10 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>22</v>
@@ -721,10 +729,10 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>23</v>
@@ -765,10 +773,10 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>24</v>
@@ -809,10 +817,10 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>25</v>
@@ -836,7 +844,7 @@
         <v>17</v>
       </c>
       <c r="K5" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -853,10 +861,10 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>22</v>
@@ -880,7 +888,7 @@
         <v>7</v>
       </c>
       <c r="K6" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="L6">
         <v>6.5</v>
@@ -897,10 +905,10 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>23</v>
@@ -924,7 +932,7 @@
         <v>15</v>
       </c>
       <c r="K7" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="L7">
         <v>3.2</v>
@@ -941,10 +949,10 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>24</v>
@@ -968,7 +976,7 @@
         <v>16</v>
       </c>
       <c r="K8" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="L8">
         <v>0.01</v>
@@ -985,10 +993,10 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>25</v>
@@ -1012,7 +1020,7 @@
         <v>17</v>
       </c>
       <c r="K9" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="L9">
         <v>3.2</v>
@@ -1029,16 +1037,16 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>32</v>

</xml_diff>